<commit_message>
updating the code to create the master datasheet for actigard
</commit_message>
<xml_diff>
--- a/data/rrv_ipm_master.xlsx
+++ b/data/rrv_ipm_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/afife_ufl_edu/Documents/Dissertation/Manuscript &amp; Data/ipm_trials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/afife_ufl_edu/Documents/DISSERTATION/MANUSCRIPT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{69ABD2D4-04A3-44DE-92CF-49550FA4D227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="114_{69ABD2D4-04A3-44DE-92CF-49550FA4D227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE0F86E-6ECF-49E8-9AFB-2A6AAA1D76C7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1204,11 +1204,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I486"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>